<commit_message>
Download de 1 arquivo XLSX completo
</commit_message>
<xml_diff>
--- a/server/uploads/SHEET.xlsx
+++ b/server/uploads/SHEET.xlsx
@@ -435,1402 +435,1402 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="str">
-        <v>507181</v>
+        <v>257496</v>
       </c>
       <c r="B2" s="2" t="str">
-        <v>79985632584</v>
+        <v>47893934184</v>
       </c>
       <c r="C2" s="2" t="str">
-        <v>Whitney Rodriguez</v>
+        <v>Adrienne Koch</v>
       </c>
       <c r="D2" s="2" t="str">
-        <v>487.94</v>
+        <v>909.27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="str">
-        <v>958842</v>
+        <v>175684</v>
       </c>
       <c r="B3" s="2" t="str">
-        <v>45092778163</v>
+        <v>35695877345</v>
       </c>
       <c r="C3" s="2" t="str">
-        <v>Jerald Rath</v>
+        <v>Darren Frami</v>
       </c>
       <c r="D3" s="2" t="str">
-        <v>721.34</v>
+        <v>539.93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="str">
-        <v>717476</v>
+        <v>548646</v>
       </c>
       <c r="B4" s="2" t="str">
-        <v>67869317950</v>
+        <v>30691235535</v>
       </c>
       <c r="C4" s="2" t="str">
-        <v>Gary Walter</v>
+        <v>Mrs. Raymond Beatty</v>
       </c>
       <c r="D4" s="2" t="str">
-        <v>898.16</v>
+        <v>25.02</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="str">
-        <v>377209</v>
+        <v>129120</v>
       </c>
       <c r="B5" s="2" t="str">
-        <v>51847724383</v>
+        <v>76095139561</v>
       </c>
       <c r="C5" s="2" t="str">
-        <v>Noah Trantow III</v>
+        <v>Franklin Daugherty</v>
       </c>
       <c r="D5" s="2" t="str">
-        <v>60.95</v>
+        <v>74.07</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="str">
-        <v>779246</v>
+        <v>231701</v>
       </c>
       <c r="B6" s="2" t="str">
-        <v>47876954544</v>
+        <v>53839472471</v>
       </c>
       <c r="C6" s="2" t="str">
-        <v>Miguel Block</v>
+        <v>Thelma Considine DVM</v>
       </c>
       <c r="D6" s="2" t="str">
-        <v>723.88</v>
+        <v>397.56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="str">
-        <v>319495</v>
+        <v>433087</v>
       </c>
       <c r="B7" s="2" t="str">
-        <v>48389437212</v>
+        <v>94541181088</v>
       </c>
       <c r="C7" s="2" t="str">
-        <v>George Yost</v>
+        <v>Kristopher Upton</v>
       </c>
       <c r="D7" s="2" t="str">
-        <v>759.40</v>
+        <v>396.70</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="str">
-        <v>865692</v>
+        <v>735809</v>
       </c>
       <c r="B8" s="2" t="str">
-        <v>91492152353</v>
+        <v>33363707270</v>
       </c>
       <c r="C8" s="2" t="str">
-        <v>Mr. Elsa Frami</v>
+        <v>Isabel Donnelly</v>
       </c>
       <c r="D8" s="2" t="str">
-        <v>804.28</v>
+        <v>547.33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="str">
-        <v>677206</v>
+        <v>361148</v>
       </c>
       <c r="B9" s="2" t="str">
-        <v>59538043942</v>
+        <v>90455496101</v>
       </c>
       <c r="C9" s="2" t="str">
-        <v>Percy Lynch</v>
+        <v>Roger Mitchell</v>
       </c>
       <c r="D9" s="2" t="str">
-        <v>598.55</v>
+        <v>870.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="str">
-        <v>431268</v>
+        <v>150933</v>
       </c>
       <c r="B10" s="2" t="str">
-        <v>67358670686</v>
+        <v>19184546195</v>
       </c>
       <c r="C10" s="2" t="str">
-        <v>Miss Velma Kunze</v>
+        <v>Ora Blanda</v>
       </c>
       <c r="D10" s="2" t="str">
-        <v>857.58</v>
+        <v>474.33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="str">
-        <v>652246</v>
+        <v>263199</v>
       </c>
       <c r="B11" s="2" t="str">
-        <v>75281977374</v>
+        <v>94481562892</v>
       </c>
       <c r="C11" s="2" t="str">
-        <v>Marianne Fadel</v>
+        <v>Tyler Stoltenberg</v>
       </c>
       <c r="D11" s="2" t="str">
-        <v>435.06</v>
+        <v>874.22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="str">
-        <v>819278</v>
+        <v>185709</v>
       </c>
       <c r="B12" s="2" t="str">
-        <v>87986604310</v>
+        <v>71539475000</v>
       </c>
       <c r="C12" s="2" t="str">
-        <v>Carmen White</v>
+        <v>Viola Walter</v>
       </c>
       <c r="D12" s="2" t="str">
-        <v>24.49</v>
+        <v>346.78</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="str">
-        <v>985378</v>
+        <v>501272</v>
       </c>
       <c r="B13" s="2" t="str">
-        <v>96765252528</v>
+        <v>63850984512</v>
       </c>
       <c r="C13" s="2" t="str">
-        <v>Sue Medhurst</v>
+        <v>Chad Doyle</v>
       </c>
       <c r="D13" s="2" t="str">
-        <v>262.90</v>
+        <v>423.03</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="str">
-        <v>596563</v>
+        <v>500227</v>
       </c>
       <c r="B14" s="2" t="str">
-        <v>44206394325</v>
+        <v>08071119640</v>
       </c>
       <c r="C14" s="2" t="str">
-        <v>Michelle Gulgowski</v>
+        <v>Beatrice Rowe</v>
       </c>
       <c r="D14" s="2" t="str">
-        <v>192.60</v>
+        <v>50.72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="str">
-        <v>518391</v>
+        <v>713595</v>
       </c>
       <c r="B15" s="2" t="str">
-        <v>65941377775</v>
+        <v>67018747027</v>
       </c>
       <c r="C15" s="2" t="str">
-        <v>Bert Lemke</v>
+        <v>Billie Fadel</v>
       </c>
       <c r="D15" s="2" t="str">
-        <v>760.43</v>
+        <v>66.29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="str">
-        <v>387840</v>
+        <v>779087</v>
       </c>
       <c r="B16" s="2" t="str">
-        <v>21984341391</v>
+        <v>58398339594</v>
       </c>
       <c r="C16" s="2" t="str">
-        <v>Terri Block</v>
+        <v>Rodney Crona</v>
       </c>
       <c r="D16" s="2" t="str">
-        <v>243.69</v>
+        <v>784.92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="str">
-        <v>481260</v>
+        <v>697489</v>
       </c>
       <c r="B17" s="2" t="str">
-        <v>98665443016</v>
+        <v>29113921988</v>
       </c>
       <c r="C17" s="2" t="str">
-        <v>Ervin Upton</v>
+        <v>Terry O'Conner</v>
       </c>
       <c r="D17" s="2" t="str">
-        <v>160.04</v>
+        <v>693.99</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="str">
-        <v>559644</v>
+        <v>433918</v>
       </c>
       <c r="B18" s="2" t="str">
-        <v>03424426866</v>
+        <v>18597189895</v>
       </c>
       <c r="C18" s="2" t="str">
-        <v>Samantha D'Amore</v>
+        <v>Phillip Daniel</v>
       </c>
       <c r="D18" s="2" t="str">
-        <v>251.88</v>
+        <v>779.84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="str">
-        <v>233488</v>
+        <v>292460</v>
       </c>
       <c r="B19" s="2" t="str">
-        <v>40594402467</v>
+        <v>74999159527</v>
       </c>
       <c r="C19" s="2" t="str">
-        <v>Alejandro Cole</v>
+        <v>Whitney Auer</v>
       </c>
       <c r="D19" s="2" t="str">
-        <v>98.01</v>
+        <v>465.06</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="str">
-        <v>652760</v>
+        <v>667587</v>
       </c>
       <c r="B20" s="2" t="str">
-        <v>82166199130</v>
+        <v>74106796854</v>
       </c>
       <c r="C20" s="2" t="str">
-        <v>Mrs. Melba Spencer</v>
+        <v>Vernon Stark</v>
       </c>
       <c r="D20" s="2" t="str">
-        <v>95.28</v>
+        <v>555.50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="str">
-        <v>228533</v>
+        <v>108996</v>
       </c>
       <c r="B21" s="2" t="str">
-        <v>97500731050</v>
+        <v>98829649132</v>
       </c>
       <c r="C21" s="2" t="str">
-        <v>Roman Sporer</v>
+        <v>Ms. Shelly Lebsack</v>
       </c>
       <c r="D21" s="2" t="str">
-        <v>563.52</v>
+        <v>234.20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="str">
-        <v>843867</v>
+        <v>536983</v>
       </c>
       <c r="B22" s="2" t="str">
-        <v>21817255415</v>
+        <v>14781632297</v>
       </c>
       <c r="C22" s="2" t="str">
-        <v>Mrs. Guadalupe Carroll</v>
+        <v>Florence Dicki</v>
       </c>
       <c r="D22" s="2" t="str">
-        <v>728.11</v>
+        <v>508.86</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="str">
-        <v>460918</v>
+        <v>297156</v>
       </c>
       <c r="B23" s="2" t="str">
-        <v>41725724306</v>
+        <v>56628023926</v>
       </c>
       <c r="C23" s="2" t="str">
-        <v>Dr. Mathew Ullrich</v>
+        <v>Carroll Homenick</v>
       </c>
       <c r="D23" s="2" t="str">
-        <v>592.83</v>
+        <v>948.86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="str">
-        <v>152670</v>
+        <v>511699</v>
       </c>
       <c r="B24" s="2" t="str">
-        <v>96667547104</v>
+        <v>26433986751</v>
       </c>
       <c r="C24" s="2" t="str">
-        <v>Ross Torp</v>
+        <v>Marvin Walsh</v>
       </c>
       <c r="D24" s="2" t="str">
-        <v>446.42</v>
+        <v>243.39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="str">
-        <v>485675</v>
+        <v>558615</v>
       </c>
       <c r="B25" s="2" t="str">
-        <v>44319717818</v>
+        <v>10362169402</v>
       </c>
       <c r="C25" s="2" t="str">
-        <v>Marc Bogan</v>
+        <v>Mrs. Melanie Hickle</v>
       </c>
       <c r="D25" s="2" t="str">
-        <v>349.63</v>
+        <v>501.75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="str">
-        <v>175137</v>
+        <v>799275</v>
       </c>
       <c r="B26" s="2" t="str">
-        <v>00942503008</v>
+        <v>30358589091</v>
       </c>
       <c r="C26" s="2" t="str">
-        <v>Homer Satterfield</v>
+        <v>Nora Little</v>
       </c>
       <c r="D26" s="2" t="str">
-        <v>95.90</v>
+        <v>867.76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="str">
-        <v>654873</v>
+        <v>427514</v>
       </c>
       <c r="B27" s="2" t="str">
-        <v>19332891143</v>
+        <v>01345441094</v>
       </c>
       <c r="C27" s="2" t="str">
-        <v>Ernest Mraz IV</v>
+        <v>May Reinger</v>
       </c>
       <c r="D27" s="2" t="str">
-        <v>889.99</v>
+        <v>86.78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="str">
-        <v>446157</v>
+        <v>976044</v>
       </c>
       <c r="B28" s="2" t="str">
-        <v>27786070201</v>
+        <v>86072475719</v>
       </c>
       <c r="C28" s="2" t="str">
-        <v>Herbert McKenzie DDS</v>
+        <v>Joann Hintz</v>
       </c>
       <c r="D28" s="2" t="str">
-        <v>870.94</v>
+        <v>577.25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="str">
-        <v>578402</v>
+        <v>276395</v>
       </c>
       <c r="B29" s="2" t="str">
-        <v>26928401738</v>
+        <v>17418089555</v>
       </c>
       <c r="C29" s="2" t="str">
-        <v>Stephanie Walsh</v>
+        <v>Shawna Terry</v>
       </c>
       <c r="D29" s="2" t="str">
-        <v>100.62</v>
+        <v>594.94</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="str">
-        <v>934043</v>
+        <v>831892</v>
       </c>
       <c r="B30" s="2" t="str">
-        <v>65196112520</v>
+        <v>60512413945</v>
       </c>
       <c r="C30" s="2" t="str">
-        <v>Gerardo Larkin</v>
+        <v>Natasha Bergstrom</v>
       </c>
       <c r="D30" s="2" t="str">
-        <v>624.12</v>
+        <v>318.65</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="str">
-        <v>851828</v>
+        <v>625590</v>
       </c>
       <c r="B31" s="2" t="str">
-        <v>15899034240</v>
+        <v>32579750660</v>
       </c>
       <c r="C31" s="2" t="str">
-        <v>Yvette Glover</v>
+        <v>Barbara Daniel</v>
       </c>
       <c r="D31" s="2" t="str">
-        <v>659.23</v>
+        <v>988.19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="str">
-        <v>727107</v>
+        <v>929889</v>
       </c>
       <c r="B32" s="2" t="str">
-        <v>74169238144</v>
+        <v>11456620320</v>
       </c>
       <c r="C32" s="2" t="str">
-        <v>Mike Collins</v>
+        <v>Eva Marvin III</v>
       </c>
       <c r="D32" s="2" t="str">
-        <v>940.75</v>
+        <v>214.38</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="str">
-        <v>895630</v>
+        <v>468940</v>
       </c>
       <c r="B33" s="2" t="str">
-        <v>15051983622</v>
+        <v>11989618069</v>
       </c>
       <c r="C33" s="2" t="str">
-        <v>Noel Cummings</v>
+        <v>Jeremiah Gutmann</v>
       </c>
       <c r="D33" s="2" t="str">
-        <v>852.24</v>
+        <v>24.40</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="str">
-        <v>350849</v>
+        <v>546407</v>
       </c>
       <c r="B34" s="2" t="str">
-        <v>56872975686</v>
+        <v>54812297411</v>
       </c>
       <c r="C34" s="2" t="str">
-        <v>Brad Kozey</v>
+        <v>Joey Bahringer</v>
       </c>
       <c r="D34" s="2" t="str">
-        <v>382.63</v>
+        <v>787.25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="str">
-        <v>631858</v>
+        <v>539785</v>
       </c>
       <c r="B35" s="2" t="str">
-        <v>52939570951</v>
+        <v>67945914249</v>
       </c>
       <c r="C35" s="2" t="str">
-        <v>Terrence Crona</v>
+        <v>Felix Osinski</v>
       </c>
       <c r="D35" s="2" t="str">
-        <v>143.67</v>
+        <v>113.67</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="str">
-        <v>244346</v>
+        <v>792705</v>
       </c>
       <c r="B36" s="2" t="str">
-        <v>46176584367</v>
+        <v>80622482416</v>
       </c>
       <c r="C36" s="2" t="str">
-        <v>Anthony Bashirian</v>
+        <v>Deborah Prosacco</v>
       </c>
       <c r="D36" s="2" t="str">
-        <v>411.73</v>
+        <v>601.93</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="str">
-        <v>312813</v>
+        <v>367738</v>
       </c>
       <c r="B37" s="2" t="str">
-        <v>12977329804</v>
+        <v>05451268516</v>
       </c>
       <c r="C37" s="2" t="str">
-        <v>Charlene Blanda</v>
+        <v>Wendell Watsica</v>
       </c>
       <c r="D37" s="2" t="str">
-        <v>395.83</v>
+        <v>58.16</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="str">
-        <v>894798</v>
+        <v>178762</v>
       </c>
       <c r="B38" s="2" t="str">
-        <v>90691207302</v>
+        <v>48667392414</v>
       </c>
       <c r="C38" s="2" t="str">
-        <v>Heather Lebsack</v>
+        <v>Omar Satterfield</v>
       </c>
       <c r="D38" s="2" t="str">
-        <v>276.49</v>
+        <v>92.84</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="str">
-        <v>803551</v>
+        <v>595152</v>
       </c>
       <c r="B39" s="2" t="str">
-        <v>03835241054</v>
+        <v>74743675440</v>
       </c>
       <c r="C39" s="2" t="str">
-        <v>Dale Farrell V</v>
+        <v>Mr. Gary McCullough</v>
       </c>
       <c r="D39" s="2" t="str">
-        <v>194.01</v>
+        <v>448.43</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="str">
-        <v>535128</v>
+        <v>852948</v>
       </c>
       <c r="B40" s="2" t="str">
-        <v>38776104128</v>
+        <v>35524392873</v>
       </c>
       <c r="C40" s="2" t="str">
-        <v>Belinda Larkin</v>
+        <v>Tommy Hirthe</v>
       </c>
       <c r="D40" s="2" t="str">
-        <v>70.01</v>
+        <v>19.96</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="str">
-        <v>971277</v>
+        <v>991941</v>
       </c>
       <c r="B41" s="2" t="str">
-        <v>84082450950</v>
+        <v>82026056130</v>
       </c>
       <c r="C41" s="2" t="str">
-        <v>Gene Halvorson</v>
+        <v>Dewey Dickinson</v>
       </c>
       <c r="D41" s="2" t="str">
-        <v>267.94</v>
+        <v>716.41</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="str">
-        <v>480221</v>
+        <v>594965</v>
       </c>
       <c r="B42" s="2" t="str">
-        <v>23102306667</v>
+        <v>57812726148</v>
       </c>
       <c r="C42" s="2" t="str">
-        <v>Samantha Botsford</v>
+        <v>Jaime Collins</v>
       </c>
       <c r="D42" s="2" t="str">
-        <v>332.00</v>
+        <v>716.76</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="str">
-        <v>124832</v>
+        <v>190925</v>
       </c>
       <c r="B43" s="2" t="str">
-        <v>70648488495</v>
+        <v>37744095060</v>
       </c>
       <c r="C43" s="2" t="str">
-        <v>Eloise Sporer</v>
+        <v>John Hills</v>
       </c>
       <c r="D43" s="2" t="str">
-        <v>57.98</v>
+        <v>516.27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="str">
-        <v>101208</v>
+        <v>747112</v>
       </c>
       <c r="B44" s="2" t="str">
-        <v>12637485750</v>
+        <v>93222186644</v>
       </c>
       <c r="C44" s="2" t="str">
-        <v>Mr. Randolph Satterfield</v>
+        <v>Miss Irma Volkman</v>
       </c>
       <c r="D44" s="2" t="str">
-        <v>751.00</v>
+        <v>986.90</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="str">
-        <v>996770</v>
+        <v>388295</v>
       </c>
       <c r="B45" s="2" t="str">
-        <v>10491457325</v>
+        <v>22640538890</v>
       </c>
       <c r="C45" s="2" t="str">
-        <v>Ms. Bernard Marquardt</v>
+        <v>Rolando Bins</v>
       </c>
       <c r="D45" s="2" t="str">
-        <v>920.83</v>
+        <v>692.61</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="str">
-        <v>710368</v>
+        <v>954756</v>
       </c>
       <c r="B46" s="2" t="str">
-        <v>31023672921</v>
+        <v>16519577777</v>
       </c>
       <c r="C46" s="2" t="str">
-        <v>Della Bednar</v>
+        <v>Shelia Morissette Sr.</v>
       </c>
       <c r="D46" s="2" t="str">
-        <v>831.14</v>
+        <v>286.11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="str">
-        <v>221661</v>
+        <v>739310</v>
       </c>
       <c r="B47" s="2" t="str">
-        <v>73403820837</v>
+        <v>89035108825</v>
       </c>
       <c r="C47" s="2" t="str">
-        <v>Erin Barton</v>
+        <v>Mrs. Herbert Blick</v>
       </c>
       <c r="D47" s="2" t="str">
-        <v>607.59</v>
+        <v>353.98</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="str">
-        <v>812730</v>
+        <v>762543</v>
       </c>
       <c r="B48" s="2" t="str">
-        <v>01015760330</v>
+        <v>50855004298</v>
       </c>
       <c r="C48" s="2" t="str">
-        <v>Noah Ryan</v>
+        <v>Nichole Erdman</v>
       </c>
       <c r="D48" s="2" t="str">
-        <v>464.67</v>
+        <v>952.57</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="str">
-        <v>442616</v>
+        <v>339400</v>
       </c>
       <c r="B49" s="2" t="str">
-        <v>09335847152</v>
+        <v>06677959742</v>
       </c>
       <c r="C49" s="2" t="str">
-        <v>Matthew Bauch</v>
+        <v>Miss Muriel Rolfson</v>
       </c>
       <c r="D49" s="2" t="str">
-        <v>380.30</v>
+        <v>750.95</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="str">
-        <v>168580</v>
+        <v>972087</v>
       </c>
       <c r="B50" s="2" t="str">
-        <v>27537701022</v>
+        <v>25125861912</v>
       </c>
       <c r="C50" s="2" t="str">
-        <v>Jessica Legros</v>
+        <v>Nick Fritsch DDS</v>
       </c>
       <c r="D50" s="2" t="str">
-        <v>753.45</v>
+        <v>927.47</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="str">
-        <v>392565</v>
+        <v>926100</v>
       </c>
       <c r="B51" s="2" t="str">
-        <v>96067345910</v>
+        <v>71397129166</v>
       </c>
       <c r="C51" s="2" t="str">
-        <v>Teresa Dicki</v>
+        <v>Jeremy Bode</v>
       </c>
       <c r="D51" s="2" t="str">
-        <v>424.19</v>
+        <v>391.90</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="str">
-        <v>299124</v>
+        <v>460661</v>
       </c>
       <c r="B52" s="2" t="str">
-        <v>64775481470</v>
+        <v>39447060483</v>
       </c>
       <c r="C52" s="2" t="str">
-        <v>Jaime Monahan</v>
+        <v>Adrian Morar III</v>
       </c>
       <c r="D52" s="2" t="str">
-        <v>100.79</v>
+        <v>152.85</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="str">
-        <v>574829</v>
+        <v>207228</v>
       </c>
       <c r="B53" s="2" t="str">
-        <v>29847347317</v>
+        <v>35682113398</v>
       </c>
       <c r="C53" s="2" t="str">
-        <v>Doreen Doyle</v>
+        <v>Willard Konopelski</v>
       </c>
       <c r="D53" s="2" t="str">
-        <v>636.16</v>
+        <v>976.53</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="str">
-        <v>271943</v>
+        <v>990985</v>
       </c>
       <c r="B54" s="2" t="str">
-        <v>45081444969</v>
+        <v>93331357999</v>
       </c>
       <c r="C54" s="2" t="str">
-        <v>Gustavo O'Kon</v>
+        <v>Roman Kulas</v>
       </c>
       <c r="D54" s="2" t="str">
-        <v>61.02</v>
+        <v>687.05</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="str">
-        <v>583853</v>
+        <v>690617</v>
       </c>
       <c r="B55" s="2" t="str">
-        <v>29897809796</v>
+        <v>19887614226</v>
       </c>
       <c r="C55" s="2" t="str">
-        <v>Mrs. Jamie Harber</v>
+        <v>Mrs. Bobby Carroll</v>
       </c>
       <c r="D55" s="2" t="str">
-        <v>25.24</v>
+        <v>292.75</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="str">
-        <v>299511</v>
+        <v>828488</v>
       </c>
       <c r="B56" s="2" t="str">
-        <v>18610386387</v>
+        <v>02561944373</v>
       </c>
       <c r="C56" s="2" t="str">
-        <v>Juana Parker</v>
+        <v>Beverly Stiedemann PhD</v>
       </c>
       <c r="D56" s="2" t="str">
-        <v>318.46</v>
+        <v>924.24</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="str">
-        <v>637600</v>
+        <v>849498</v>
       </c>
       <c r="B57" s="2" t="str">
-        <v>80840088729</v>
+        <v>01608087075</v>
       </c>
       <c r="C57" s="2" t="str">
-        <v>Ben Torphy</v>
+        <v>Billie Hansen</v>
       </c>
       <c r="D57" s="2" t="str">
-        <v>840.30</v>
+        <v>68.47</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="str">
-        <v>566774</v>
+        <v>134103</v>
       </c>
       <c r="B58" s="2" t="str">
-        <v>22836451372</v>
+        <v>16764445253</v>
       </c>
       <c r="C58" s="2" t="str">
-        <v>Andrew Wunsch</v>
+        <v>Linda Kulas</v>
       </c>
       <c r="D58" s="2" t="str">
-        <v>666.17</v>
+        <v>469.59</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="str">
-        <v>641218</v>
+        <v>443144</v>
       </c>
       <c r="B59" s="2" t="str">
-        <v>76072501484</v>
+        <v>52632167772</v>
       </c>
       <c r="C59" s="2" t="str">
-        <v>Bernice Upton</v>
+        <v>Blanca Jaskolski</v>
       </c>
       <c r="D59" s="2" t="str">
-        <v>819.84</v>
+        <v>195.30</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="str">
-        <v>206717</v>
+        <v>978468</v>
       </c>
       <c r="B60" s="2" t="str">
-        <v>94237476307</v>
+        <v>38833701866</v>
       </c>
       <c r="C60" s="2" t="str">
-        <v>Wallace Upton</v>
+        <v>Otis Hermann</v>
       </c>
       <c r="D60" s="2" t="str">
-        <v>597.40</v>
+        <v>673.34</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="str">
-        <v>159873</v>
+        <v>536347</v>
       </c>
       <c r="B61" s="2" t="str">
-        <v>51204974413</v>
+        <v>87561722774</v>
       </c>
       <c r="C61" s="2" t="str">
-        <v>Jenny Hagenes</v>
+        <v>Bernard O'Kon</v>
       </c>
       <c r="D61" s="2" t="str">
-        <v>643.95</v>
+        <v>124.96</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="str">
-        <v>880505</v>
+        <v>143507</v>
       </c>
       <c r="B62" s="2" t="str">
-        <v>57150393212</v>
+        <v>41590203973</v>
       </c>
       <c r="C62" s="2" t="str">
-        <v>Tiffany Rodriguez</v>
+        <v>Jeannette Green</v>
       </c>
       <c r="D62" s="2" t="str">
-        <v>378.32</v>
+        <v>401.75</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="str">
-        <v>379853</v>
+        <v>901619</v>
       </c>
       <c r="B63" s="2" t="str">
-        <v>33886268688</v>
+        <v>41711288341</v>
       </c>
       <c r="C63" s="2" t="str">
-        <v>Ron Lang</v>
+        <v>Edith Conn</v>
       </c>
       <c r="D63" s="2" t="str">
-        <v>127.56</v>
+        <v>727.68</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="str">
-        <v>818020</v>
+        <v>817345</v>
       </c>
       <c r="B64" s="2" t="str">
-        <v>55171852698</v>
+        <v>74743042397</v>
       </c>
       <c r="C64" s="2" t="str">
-        <v>Sonja Waters</v>
+        <v>Kendra Howell DVM</v>
       </c>
       <c r="D64" s="2" t="str">
-        <v>392.60</v>
+        <v>420.66</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="str">
-        <v>421661</v>
+        <v>961497</v>
       </c>
       <c r="B65" s="2" t="str">
-        <v>69379204744</v>
+        <v>24713626201</v>
       </c>
       <c r="C65" s="2" t="str">
-        <v>Leigh Emmerich</v>
+        <v>Josephine Franecki</v>
       </c>
       <c r="D65" s="2" t="str">
-        <v>699.65</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="str">
-        <v>472327</v>
+        <v>723785</v>
       </c>
       <c r="B66" s="2" t="str">
-        <v>30907756881</v>
+        <v>28490286273</v>
       </c>
       <c r="C66" s="2" t="str">
-        <v>Jacob Ryan</v>
+        <v>Edmund Huels Jr.</v>
       </c>
       <c r="D66" s="2" t="str">
-        <v>870.65</v>
+        <v>538.49</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="str">
-        <v>689399</v>
+        <v>373873</v>
       </c>
       <c r="B67" s="2" t="str">
-        <v>58428094699</v>
+        <v>59258743887</v>
       </c>
       <c r="C67" s="2" t="str">
-        <v>Randy Bosco</v>
+        <v>Jay Dach</v>
       </c>
       <c r="D67" s="2" t="str">
-        <v>531.59</v>
+        <v>662.88</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="str">
-        <v>670258</v>
+        <v>132714</v>
       </c>
       <c r="B68" s="2" t="str">
-        <v>83172899461</v>
+        <v>10408676159</v>
       </c>
       <c r="C68" s="2" t="str">
-        <v>Mary Huel</v>
+        <v>Charlene Leannon</v>
       </c>
       <c r="D68" s="2" t="str">
-        <v>238.59</v>
+        <v>808.00</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="str">
-        <v>914426</v>
+        <v>258377</v>
       </c>
       <c r="B69" s="2" t="str">
-        <v>75871935370</v>
+        <v>32395437802</v>
       </c>
       <c r="C69" s="2" t="str">
-        <v>June Bartoletti</v>
+        <v>Rachel Heaney Sr.</v>
       </c>
       <c r="D69" s="2" t="str">
-        <v>244.79</v>
+        <v>63.69</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="str">
-        <v>302146</v>
+        <v>515261</v>
       </c>
       <c r="B70" s="2" t="str">
-        <v>19466612604</v>
+        <v>25177909410</v>
       </c>
       <c r="C70" s="2" t="str">
-        <v>Donnie Wiegand</v>
+        <v>Madeline Steuber</v>
       </c>
       <c r="D70" s="2" t="str">
-        <v>414.35</v>
+        <v>70.27</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="str">
-        <v>276212</v>
+        <v>453589</v>
       </c>
       <c r="B71" s="2" t="str">
-        <v>09227232402</v>
+        <v>26095698983</v>
       </c>
       <c r="C71" s="2" t="str">
-        <v>Archie Steuber</v>
+        <v>Flora Graham</v>
       </c>
       <c r="D71" s="2" t="str">
-        <v>812.06</v>
+        <v>149.12</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="str">
-        <v>796162</v>
+        <v>289477</v>
       </c>
       <c r="B72" s="2" t="str">
-        <v>51707554003</v>
+        <v>13417169381</v>
       </c>
       <c r="C72" s="2" t="str">
-        <v>Mrs. Tony Tromp</v>
+        <v>Cesar Bode</v>
       </c>
       <c r="D72" s="2" t="str">
-        <v>298.27</v>
+        <v>717.14</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="str">
-        <v>464326</v>
+        <v>503408</v>
       </c>
       <c r="B73" s="2" t="str">
-        <v>69211286306</v>
+        <v>60156299360</v>
       </c>
       <c r="C73" s="2" t="str">
-        <v>Billie Cole II</v>
+        <v>Jermaine Bergstrom</v>
       </c>
       <c r="D73" s="2" t="str">
-        <v>91.76</v>
+        <v>140.39</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="str">
-        <v>381186</v>
+        <v>982573</v>
       </c>
       <c r="B74" s="2" t="str">
-        <v>19362901290</v>
+        <v>11977858375</v>
       </c>
       <c r="C74" s="2" t="str">
-        <v>Lynne Koelpin</v>
+        <v>Darrell Conn</v>
       </c>
       <c r="D74" s="2" t="str">
-        <v>331.60</v>
+        <v>458.24</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="str">
-        <v>768693</v>
+        <v>579704</v>
       </c>
       <c r="B75" s="2" t="str">
-        <v>61973773385</v>
+        <v>43741296627</v>
       </c>
       <c r="C75" s="2" t="str">
-        <v>Lowell Luettgen II</v>
+        <v>Joy Dare</v>
       </c>
       <c r="D75" s="2" t="str">
-        <v>15.82</v>
+        <v>950.40</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="str">
-        <v>357692</v>
+        <v>128276</v>
       </c>
       <c r="B76" s="2" t="str">
-        <v>38224438577</v>
+        <v>40022241859</v>
       </c>
       <c r="C76" s="2" t="str">
-        <v>Darlene Yundt</v>
+        <v>Orville Feeney</v>
       </c>
       <c r="D76" s="2" t="str">
-        <v>23.21</v>
+        <v>665.14</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="str">
-        <v>424639</v>
+        <v>858130</v>
       </c>
       <c r="B77" s="2" t="str">
-        <v>63256606366</v>
+        <v>41421694983</v>
       </c>
       <c r="C77" s="2" t="str">
-        <v>Curtis West</v>
+        <v>Frederick Jacobson</v>
       </c>
       <c r="D77" s="2" t="str">
-        <v>596.74</v>
+        <v>420.58</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="str">
-        <v>683101</v>
+        <v>866313</v>
       </c>
       <c r="B78" s="2" t="str">
-        <v>86814838927</v>
+        <v>28709289454</v>
       </c>
       <c r="C78" s="2" t="str">
-        <v>Louise Witting MD</v>
+        <v>Debra Dicki</v>
       </c>
       <c r="D78" s="2" t="str">
-        <v>823.38</v>
+        <v>120.78</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="str">
-        <v>275829</v>
+        <v>272094</v>
       </c>
       <c r="B79" s="2" t="str">
-        <v>27145689097</v>
+        <v>50383872585</v>
       </c>
       <c r="C79" s="2" t="str">
-        <v>Charlie Johnston</v>
+        <v>Nora Quitzon</v>
       </c>
       <c r="D79" s="2" t="str">
-        <v>808.46</v>
+        <v>989.30</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="str">
-        <v>693018</v>
+        <v>399985</v>
       </c>
       <c r="B80" s="2" t="str">
-        <v>75480286846</v>
+        <v>65535907074</v>
       </c>
       <c r="C80" s="2" t="str">
-        <v>Candice Bauch</v>
+        <v>Kristy Hyatt</v>
       </c>
       <c r="D80" s="2" t="str">
-        <v>842.25</v>
+        <v>951.46</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="str">
-        <v>311958</v>
+        <v>510462</v>
       </c>
       <c r="B81" s="2" t="str">
-        <v>85763617977</v>
+        <v>14746183902</v>
       </c>
       <c r="C81" s="2" t="str">
-        <v>Janice Hessel II</v>
+        <v>Jennie Greenholt</v>
       </c>
       <c r="D81" s="2" t="str">
-        <v>84.54</v>
+        <v>320.66</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="str">
-        <v>642975</v>
+        <v>200424</v>
       </c>
       <c r="B82" s="2" t="str">
-        <v>48794395430</v>
+        <v>76646418753</v>
       </c>
       <c r="C82" s="2" t="str">
-        <v>Krystal Prosacco</v>
+        <v>Dr. Darren Bergstrom</v>
       </c>
       <c r="D82" s="2" t="str">
-        <v>918.51</v>
+        <v>366.54</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="str">
-        <v>529640</v>
+        <v>348246</v>
       </c>
       <c r="B83" s="2" t="str">
-        <v>41955043794</v>
+        <v>31410276680</v>
       </c>
       <c r="C83" s="2" t="str">
-        <v>May Fahey</v>
+        <v>Bonnie Raynor</v>
       </c>
       <c r="D83" s="2" t="str">
-        <v>10.97</v>
+        <v>493.16</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="str">
-        <v>727547</v>
+        <v>710832</v>
       </c>
       <c r="B84" s="2" t="str">
-        <v>52355708135</v>
+        <v>72584808757</v>
       </c>
       <c r="C84" s="2" t="str">
-        <v>Miss Hugh Swaniawski</v>
+        <v>Lisa Cormier</v>
       </c>
       <c r="D84" s="2" t="str">
-        <v>782.37</v>
+        <v>314.69</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="str">
-        <v>709946</v>
+        <v>793321</v>
       </c>
       <c r="B85" s="2" t="str">
-        <v>14601470902</v>
+        <v>36856406298</v>
       </c>
       <c r="C85" s="2" t="str">
-        <v>Mathew Waelchi</v>
+        <v>Ms. Hilda Skiles</v>
       </c>
       <c r="D85" s="2" t="str">
-        <v>665.29</v>
+        <v>407.25</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="str">
-        <v>619840</v>
+        <v>897880</v>
       </c>
       <c r="B86" s="2" t="str">
-        <v>78821967355</v>
+        <v>56258704932</v>
       </c>
       <c r="C86" s="2" t="str">
-        <v>Angie Boyer</v>
+        <v>Ora Abshire</v>
       </c>
       <c r="D86" s="2" t="str">
-        <v>955.60</v>
+        <v>528.67</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="str">
-        <v>740483</v>
+        <v>672466</v>
       </c>
       <c r="B87" s="2" t="str">
-        <v>29773554299</v>
+        <v>98660323419</v>
       </c>
       <c r="C87" s="2" t="str">
-        <v>Molly Howell</v>
+        <v>Amy Reichel</v>
       </c>
       <c r="D87" s="2" t="str">
-        <v>570.53</v>
+        <v>363.66</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="str">
-        <v>672766</v>
+        <v>434806</v>
       </c>
       <c r="B88" s="2" t="str">
-        <v>41757637448</v>
+        <v>10159530676</v>
       </c>
       <c r="C88" s="2" t="str">
-        <v>Kenny Heller</v>
+        <v>Eunice Schamberger</v>
       </c>
       <c r="D88" s="2" t="str">
-        <v>350.16</v>
+        <v>731.98</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="str">
-        <v>586188</v>
+        <v>208962</v>
       </c>
       <c r="B89" s="2" t="str">
-        <v>64471960626</v>
+        <v>77720165741</v>
       </c>
       <c r="C89" s="2" t="str">
-        <v>Marvin Gislason</v>
+        <v>Clay Hermiston</v>
       </c>
       <c r="D89" s="2" t="str">
-        <v>327.83</v>
+        <v>511.80</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="str">
-        <v>630786</v>
+        <v>345001</v>
       </c>
       <c r="B90" s="2" t="str">
-        <v>02772098872</v>
+        <v>44155465764</v>
       </c>
       <c r="C90" s="2" t="str">
-        <v>Priscilla Rice</v>
+        <v>Angelina Mraz</v>
       </c>
       <c r="D90" s="2" t="str">
-        <v>19.38</v>
+        <v>52.81</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="str">
-        <v>661640</v>
+        <v>867259</v>
       </c>
       <c r="B91" s="2" t="str">
-        <v>76948233018</v>
+        <v>27359473984</v>
       </c>
       <c r="C91" s="2" t="str">
-        <v>Ms. Todd Rodriguez</v>
+        <v>Julian Kutch</v>
       </c>
       <c r="D91" s="2" t="str">
-        <v>384.24</v>
+        <v>261.26</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="str">
-        <v>955923</v>
+        <v>737583</v>
       </c>
       <c r="B92" s="2" t="str">
-        <v>30572923342</v>
+        <v>19140885351</v>
       </c>
       <c r="C92" s="2" t="str">
-        <v>Marcia Bartell</v>
+        <v>Dr. Cristina Von</v>
       </c>
       <c r="D92" s="2" t="str">
-        <v>298.99</v>
+        <v>840.35</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="str">
-        <v>720113</v>
+        <v>193647</v>
       </c>
       <c r="B93" s="2" t="str">
-        <v>86651133256</v>
+        <v>46566184167</v>
       </c>
       <c r="C93" s="2" t="str">
-        <v>Jo Stehr</v>
+        <v>David Daugherty</v>
       </c>
       <c r="D93" s="2" t="str">
-        <v>128.82</v>
+        <v>333.62</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="str">
-        <v>756991</v>
+        <v>556290</v>
       </c>
       <c r="B94" s="2" t="str">
-        <v>46474275644</v>
+        <v>56549093383</v>
       </c>
       <c r="C94" s="2" t="str">
-        <v>Myron Larkin</v>
+        <v>Bert Ziemann</v>
       </c>
       <c r="D94" s="2" t="str">
-        <v>334.40</v>
+        <v>943.67</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="str">
-        <v>728799</v>
+        <v>922502</v>
       </c>
       <c r="B95" s="2" t="str">
-        <v>22282993607</v>
+        <v>88266274565</v>
       </c>
       <c r="C95" s="2" t="str">
-        <v>Amy DuBuque</v>
+        <v>Felix Rath</v>
       </c>
       <c r="D95" s="2" t="str">
-        <v>627.64</v>
+        <v>26.44</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="str">
-        <v>203638</v>
+        <v>780201</v>
       </c>
       <c r="B96" s="2" t="str">
-        <v>40101750846</v>
+        <v>34457646030</v>
       </c>
       <c r="C96" s="2" t="str">
-        <v>Manuel Jones</v>
+        <v>Josephine Schowalter</v>
       </c>
       <c r="D96" s="2" t="str">
-        <v>543.05</v>
+        <v>308.07</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="str">
-        <v>802586</v>
+        <v>778264</v>
       </c>
       <c r="B97" s="2" t="str">
-        <v>38286349317</v>
+        <v>20769658545</v>
       </c>
       <c r="C97" s="2" t="str">
-        <v>Dr. Lorraine Hudson</v>
+        <v>Wanda Ryan</v>
       </c>
       <c r="D97" s="2" t="str">
-        <v>71.30</v>
+        <v>455.91</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="str">
-        <v>818443</v>
+        <v>624284</v>
       </c>
       <c r="B98" s="2" t="str">
-        <v>89866643864</v>
+        <v>34206962538</v>
       </c>
       <c r="C98" s="2" t="str">
-        <v>Erick Ullrich</v>
+        <v>Dr. Roland Reinger</v>
       </c>
       <c r="D98" s="2" t="str">
-        <v>658.15</v>
+        <v>652.26</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="str">
-        <v>481045</v>
+        <v>202423</v>
       </c>
       <c r="B99" s="2" t="str">
-        <v>18530626804</v>
+        <v>14926510653</v>
       </c>
       <c r="C99" s="2" t="str">
-        <v>Mr. Cecelia Dare</v>
+        <v>Alan Funk</v>
       </c>
       <c r="D99" s="2" t="str">
-        <v>692.36</v>
+        <v>851.07</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="str">
-        <v>763609</v>
+        <v>103757</v>
       </c>
       <c r="B100" s="2" t="str">
-        <v>00081940903</v>
+        <v>94978315453</v>
       </c>
       <c r="C100" s="2" t="str">
-        <v>Jeffrey Daniel</v>
+        <v>Nancy Hoeger</v>
       </c>
       <c r="D100" s="2" t="str">
-        <v>548.66</v>
+        <v>729.84</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="str">
-        <v>606012</v>
+        <v>919963</v>
       </c>
       <c r="B101" s="2" t="str">
-        <v>54589382465</v>
+        <v>00509469350</v>
       </c>
       <c r="C101" s="2" t="str">
-        <v>Rogelio McGlynn</v>
+        <v>Johnathan McLaughlin</v>
       </c>
       <c r="D101" s="2" t="str">
-        <v>713.56</v>
+        <v>968.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>